<commit_message>
Added overrides and finished scaling code
</commit_message>
<xml_diff>
--- a/RoboRIO Ports and other controls.xlsx
+++ b/RoboRIO Ports and other controls.xlsx
@@ -84,12 +84,6 @@
     <t>Intake</t>
   </si>
   <si>
-    <t>Scaler Left Lift</t>
-  </si>
-  <si>
-    <t>Scaler Right Lift</t>
-  </si>
-  <si>
     <t>DIO 0/1</t>
   </si>
   <si>
@@ -217,6 +211,12 @@
   </si>
   <si>
     <t>DIO6</t>
+  </si>
+  <si>
+    <t>Scaler Lift 1</t>
+  </si>
+  <si>
+    <t>Scaler Lift 2</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>16</v>
@@ -644,18 +644,18 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -666,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -677,7 +677,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -688,117 +688,117 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -825,52 +825,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Ports and other controls file
</commit_message>
<xml_diff>
--- a/RoboRIO Ports and other controls.xlsx
+++ b/RoboRIO Ports and other controls.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojog\Documents\GitHub\2016_STRONGHOLD_OFFICIAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kellyj\Documents\GitHub\2016_STRONGHOLD_OFFICIAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8412"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="RoboRIO Ports" sheetId="1" r:id="rId1"/>
     <sheet name="Controller Map" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>Port</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Intake Arm #2</t>
   </si>
   <si>
-    <t>Left and Right Motors</t>
-  </si>
-  <si>
     <t>Intake</t>
   </si>
   <si>
@@ -217,13 +214,25 @@
   </si>
   <si>
     <t>RefNum (Programming)</t>
+  </si>
+  <si>
+    <t>RobotDrive</t>
+  </si>
+  <si>
+    <t>Inverts</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,13 +249,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -258,17 +279,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,31 +605,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -613,10 +640,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -624,8 +654,11 @@
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -633,10 +666,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -644,21 +680,27 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -666,10 +708,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -677,10 +722,13 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -688,117 +736,123 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -818,59 +872,59 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>